<commit_message>
Made some Debug And Updated the Lessons File .xlsx
</commit_message>
<xml_diff>
--- a/assets/foglio.xlsx
+++ b/assets/foglio.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="88">
   <si>
     <t>PRIMA
 SETTIM.</t>
@@ -32,7 +32,7 @@
     <t>VENERDI' 29 Sett.</t>
   </si>
   <si>
-    <t>BOTANICA</t>
+    <t>Incontro delle matricole con il Coordinatore del corso di laurea e le manager didattiche</t>
   </si>
   <si>
     <t>MATEMATICA</t>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>ZOOLOGIA</t>
+  </si>
+  <si>
+    <t>BOTANICA</t>
+  </si>
+  <si>
+    <t>15:00</t>
   </si>
   <si>
     <t>SECONDA
@@ -278,6 +284,9 @@
     <t>VENERDI' 22 Dic.</t>
   </si>
   <si>
+    <t>zoologia</t>
+  </si>
+  <si>
     <t>Eventuali lezioni di recupero</t>
   </si>
 </sst>
@@ -325,8 +334,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFADE144"/>
-        <bgColor rgb="FFADE144"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -349,8 +358,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFADE144"/>
+        <bgColor rgb="FFADE144"/>
       </patternFill>
     </fill>
     <fill>
@@ -360,30 +369,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -399,80 +386,60 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="2" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
+    <xf borderId="2" fillId="8" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,19 +651,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.63"/>
-    <col customWidth="1" min="2" max="2" width="18.5"/>
-    <col customWidth="1" min="3" max="3" width="17.75"/>
-    <col customWidth="1" min="4" max="4" width="18.5"/>
-    <col customWidth="1" min="5" max="5" width="17.5"/>
-    <col customWidth="1" min="6" max="6" width="17.88"/>
+    <col customWidth="1" min="1" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -739,7 +700,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" ht="26.25" customHeight="1">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4">
         <v>0.375</v>
       </c>
@@ -826,11 +787,11 @@
       <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
+      <c r="C4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>8</v>
@@ -866,11 +827,11 @@
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>6</v>
+      <c r="C5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>8</v>
@@ -900,24 +861,12 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -941,23 +890,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="4">
-        <v>0.375</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -980,24 +919,14 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="4">
-        <v>0.4166666666666667</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1021,23 +950,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="4">
-        <v>0.4583333333333333</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>9</v>
-      </c>
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1061,23 +980,13 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>9</v>
-      </c>
+        <v>0.7083333333333334</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1101,22 +1010,22 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="F11" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1143,11 +1052,11 @@
       <c r="A12" s="4">
         <v>0.375</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>9</v>
+      <c r="B12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>8</v>
@@ -1183,11 +1092,11 @@
       <c r="A13" s="4">
         <v>0.4166666666666667</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>9</v>
+      <c r="B13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>8</v>
@@ -1226,11 +1135,11 @@
       <c r="B14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>6</v>
+      <c r="C14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>8</v>
@@ -1266,11 +1175,11 @@
       <c r="B15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>6</v>
+      <c r="C15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>8</v>
@@ -1328,7 +1237,9 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="4"/>
+      <c r="A17" s="4">
+        <v>0.5833333333333334</v>
+      </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -1356,7 +1267,9 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="13"/>
+      <c r="A18" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
@@ -1384,7 +1297,9 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="4"/>
+      <c r="A19" s="4">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
@@ -1412,7 +1327,9 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="4"/>
+      <c r="A20" s="4">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -1441,22 +1358,22 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="F21" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1483,8 +1400,8 @@
       <c r="A22" s="4">
         <v>0.375</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>6</v>
+      <c r="B22" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>9</v>
@@ -1523,8 +1440,8 @@
       <c r="A23" s="4">
         <v>0.4166666666666667</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>6</v>
+      <c r="B23" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>9</v>
@@ -1569,11 +1486,11 @@
       <c r="C24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>6</v>
+      <c r="D24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>9</v>
@@ -1609,11 +1526,11 @@
       <c r="C25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>6</v>
+      <c r="D25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>9</v>
@@ -1668,7 +1585,9 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="4"/>
+      <c r="A27" s="4">
+        <v>0.5833333333333334</v>
+      </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
@@ -1696,7 +1615,9 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="13"/>
+      <c r="A28" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
@@ -1724,7 +1645,9 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="4"/>
+      <c r="A29" s="4">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
@@ -1752,7 +1675,9 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="4"/>
+      <c r="A30" s="4">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
@@ -1781,22 +1706,22 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="F31" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -1823,8 +1748,8 @@
       <c r="A32" s="4">
         <v>0.375</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>6</v>
+      <c r="B32" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>9</v>
@@ -1863,8 +1788,8 @@
       <c r="A33" s="4">
         <v>0.4166666666666667</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>6</v>
+      <c r="B33" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>9</v>
@@ -1909,11 +1834,11 @@
       <c r="C34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>6</v>
+      <c r="D34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>9</v>
@@ -1949,11 +1874,11 @@
       <c r="C35" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>6</v>
+      <c r="D35" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>9</v>
@@ -2008,7 +1933,9 @@
       <c r="Z36" s="3"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="4"/>
+      <c r="A37" s="4">
+        <v>0.5833333333333334</v>
+      </c>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
@@ -2036,7 +1963,9 @@
       <c r="Z37" s="3"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="13"/>
+      <c r="A38" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
@@ -2064,7 +1993,9 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="4"/>
+      <c r="A39" s="4">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
@@ -2092,7 +2023,9 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="4"/>
+      <c r="A40" s="4">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
@@ -2121,22 +2054,22 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="F41" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -2163,13 +2096,15 @@
       <c r="A42" s="4">
         <v>0.375</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>6</v>
+      <c r="B42" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="14"/>
+      <c r="D42" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="E42" s="8" t="s">
         <v>9</v>
       </c>
@@ -2201,13 +2136,15 @@
       <c r="A43" s="4">
         <v>0.4166666666666667</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>6</v>
+      <c r="B43" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="14"/>
+      <c r="D43" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="E43" s="8" t="s">
         <v>9</v>
       </c>
@@ -2245,9 +2182,11 @@
       <c r="C44" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="14"/>
-      <c r="E44" s="5" t="s">
-        <v>6</v>
+      <c r="D44" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>9</v>
@@ -2283,9 +2222,11 @@
       <c r="C45" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="14"/>
-      <c r="E45" s="5" t="s">
-        <v>6</v>
+      <c r="D45" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>9</v>
@@ -2315,7 +2256,7 @@
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
-      <c r="D46" s="15"/>
+      <c r="D46" s="11"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="3"/>
@@ -2340,10 +2281,12 @@
       <c r="Z46" s="3"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="4"/>
+      <c r="A47" s="4">
+        <v>0.5833333333333334</v>
+      </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
-      <c r="D47" s="14"/>
+      <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
       <c r="G47" s="3"/>
@@ -2368,10 +2311,12 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="13"/>
+      <c r="A48" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
-      <c r="D48" s="14"/>
+      <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
       <c r="G48" s="3"/>
@@ -2396,10 +2341,12 @@
       <c r="Z48" s="3"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="4"/>
+      <c r="A49" s="4">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
-      <c r="D49" s="14"/>
+      <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="3"/>
@@ -2424,10 +2371,12 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="4"/>
+      <c r="A50" s="4">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
-      <c r="D50" s="14"/>
+      <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="G50" s="3"/>
@@ -2453,22 +2402,22 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="F51" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -2495,15 +2444,13 @@
       <c r="A52" s="4">
         <v>0.375</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>6</v>
+      <c r="B52" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D52" s="14"/>
       <c r="E52" s="8" t="s">
         <v>9</v>
       </c>
@@ -2535,15 +2482,13 @@
       <c r="A53" s="4">
         <v>0.4166666666666667</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>6</v>
+      <c r="B53" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D53" s="14"/>
       <c r="E53" s="8" t="s">
         <v>9</v>
       </c>
@@ -2581,11 +2526,9 @@
       <c r="C54" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>8</v>
+      <c r="D54" s="14"/>
+      <c r="E54" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>9</v>
@@ -2621,11 +2564,9 @@
       <c r="C55" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>8</v>
+      <c r="D55" s="14"/>
+      <c r="E55" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>9</v>
@@ -2655,7 +2596,7 @@
       <c r="A56" s="10"/>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
-      <c r="D56" s="16"/>
+      <c r="D56" s="14"/>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
       <c r="G56" s="3"/>
@@ -2680,10 +2621,12 @@
       <c r="Z56" s="3"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="4"/>
+      <c r="A57" s="4">
+        <v>0.5833333333333334</v>
+      </c>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
+      <c r="D57" s="14"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
       <c r="G57" s="3"/>
@@ -2708,10 +2651,12 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="13"/>
+      <c r="A58" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
+      <c r="D58" s="14"/>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
       <c r="G58" s="3"/>
@@ -2736,10 +2681,12 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="4"/>
+      <c r="A59" s="4">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
+      <c r="D59" s="14"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
       <c r="G59" s="3"/>
@@ -2764,10 +2711,12 @@
       <c r="Z59" s="3"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="4"/>
+      <c r="A60" s="4">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
+      <c r="D60" s="14"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
       <c r="G60" s="3"/>
@@ -2793,22 +2742,22 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="F61" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
@@ -2835,8 +2784,8 @@
       <c r="A62" s="4">
         <v>0.375</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>6</v>
+      <c r="B62" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>9</v>
@@ -2875,8 +2824,8 @@
       <c r="A63" s="4">
         <v>0.4166666666666667</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>6</v>
+      <c r="B63" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>9</v>
@@ -2921,8 +2870,8 @@
       <c r="C64" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>6</v>
+      <c r="D64" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>8</v>
@@ -2961,8 +2910,8 @@
       <c r="C65" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>6</v>
+      <c r="D65" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>8</v>
@@ -2995,7 +2944,7 @@
       <c r="A66" s="10"/>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
-      <c r="D66" s="16"/>
+      <c r="D66" s="12"/>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
       <c r="G66" s="3"/>
@@ -3020,7 +2969,9 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="4"/>
+      <c r="A67" s="4">
+        <v>0.5833333333333334</v>
+      </c>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
@@ -3048,7 +2999,9 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="13"/>
+      <c r="A68" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
@@ -3076,7 +3029,9 @@
       <c r="Z68" s="3"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="4"/>
+      <c r="A69" s="4">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
@@ -3104,7 +3059,9 @@
       <c r="Z69" s="3"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="4"/>
+      <c r="A70" s="4">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
       <c r="D70" s="12"/>
@@ -3133,22 +3090,22 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="F71" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
@@ -3175,8 +3132,8 @@
       <c r="A72" s="4">
         <v>0.375</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>6</v>
+      <c r="B72" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>9</v>
@@ -3215,8 +3172,8 @@
       <c r="A73" s="4">
         <v>0.4166666666666667</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>6</v>
+      <c r="B73" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>9</v>
@@ -3261,11 +3218,11 @@
       <c r="C74" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>6</v>
+      <c r="D74" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F74" s="8" t="s">
         <v>9</v>
@@ -3301,11 +3258,11 @@
       <c r="C75" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D75" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>6</v>
+      <c r="D75" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F75" s="8" t="s">
         <v>9</v>
@@ -3335,7 +3292,7 @@
       <c r="A76" s="10"/>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
-      <c r="D76" s="16"/>
+      <c r="D76" s="12"/>
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
       <c r="G76" s="3"/>
@@ -3363,21 +3320,11 @@
       <c r="A77" s="4">
         <v>0.5833333333333334</v>
       </c>
-      <c r="B77" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D77" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E77" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F77" s="17" t="s">
-        <v>58</v>
-      </c>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -3400,24 +3347,14 @@
       <c r="Z77" s="3"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="18">
-        <v>0.625</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C78" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D78" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E78" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F78" s="17" t="s">
-        <v>58</v>
-      </c>
+      <c r="A78" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
@@ -3443,21 +3380,11 @@
       <c r="A79" s="4">
         <v>0.6666666666666666</v>
       </c>
-      <c r="B79" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C79" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D79" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E79" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F79" s="17" t="s">
-        <v>58</v>
-      </c>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
@@ -3483,21 +3410,11 @@
       <c r="A80" s="4">
         <v>0.7083333333333334</v>
       </c>
-      <c r="B80" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C80" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D80" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E80" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F80" s="17" t="s">
-        <v>58</v>
-      </c>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
@@ -3521,22 +3438,22 @@
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
@@ -3563,8 +3480,8 @@
       <c r="A82" s="4">
         <v>0.375</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>6</v>
+      <c r="B82" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>9</v>
@@ -3603,8 +3520,8 @@
       <c r="A83" s="4">
         <v>0.4166666666666667</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>6</v>
+      <c r="B83" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>9</v>
@@ -3649,11 +3566,11 @@
       <c r="C84" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D84" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>8</v>
+      <c r="D84" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="F84" s="8" t="s">
         <v>9</v>
@@ -3689,11 +3606,11 @@
       <c r="C85" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D85" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>8</v>
+      <c r="D85" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="F85" s="8" t="s">
         <v>9</v>
@@ -3723,7 +3640,7 @@
       <c r="A86" s="10"/>
       <c r="B86" s="11"/>
       <c r="C86" s="11"/>
-      <c r="D86" s="16"/>
+      <c r="D86" s="12"/>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>
       <c r="G86" s="3"/>
@@ -3751,19 +3668,21 @@
       <c r="A87" s="4">
         <v>0.5833333333333334</v>
       </c>
-      <c r="B87" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C87" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D87" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E87" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F87" s="12"/>
+      <c r="B87" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E87" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F87" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
@@ -3786,22 +3705,24 @@
       <c r="Z87" s="3"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="18">
-        <v>0.625</v>
-      </c>
-      <c r="B88" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D88" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E88" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F88" s="12"/>
+      <c r="A88" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E88" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F88" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -3827,19 +3748,21 @@
       <c r="A89" s="4">
         <v>0.6666666666666666</v>
       </c>
-      <c r="B89" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C89" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D89" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E89" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F89" s="12"/>
+      <c r="B89" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E89" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F89" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -3865,19 +3788,21 @@
       <c r="A90" s="4">
         <v>0.7083333333333334</v>
       </c>
-      <c r="B90" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C90" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D90" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E90" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F90" s="12"/>
+      <c r="B90" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E90" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F90" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
@@ -3901,22 +3826,22 @@
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="F91" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D91" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F91" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
@@ -3943,8 +3868,8 @@
       <c r="A92" s="4">
         <v>0.375</v>
       </c>
-      <c r="B92" s="5" t="s">
-        <v>6</v>
+      <c r="B92" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>9</v>
@@ -3955,7 +3880,9 @@
       <c r="E92" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F92" s="14"/>
+      <c r="F92" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
@@ -3981,8 +3908,8 @@
       <c r="A93" s="4">
         <v>0.4166666666666667</v>
       </c>
-      <c r="B93" s="5" t="s">
-        <v>6</v>
+      <c r="B93" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>9</v>
@@ -3993,7 +3920,9 @@
       <c r="E93" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F93" s="14"/>
+      <c r="F93" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
@@ -4025,13 +3954,15 @@
       <c r="C94" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D94" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F94" s="14"/>
+      <c r="D94" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
@@ -4063,13 +3994,15 @@
       <c r="C95" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D95" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F95" s="14"/>
+      <c r="D95" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
@@ -4095,9 +4028,9 @@
       <c r="A96" s="10"/>
       <c r="B96" s="11"/>
       <c r="C96" s="11"/>
-      <c r="D96" s="16"/>
+      <c r="D96" s="12"/>
       <c r="E96" s="11"/>
-      <c r="F96" s="15"/>
+      <c r="F96" s="11"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
@@ -4123,19 +4056,19 @@
       <c r="A97" s="4">
         <v>0.5833333333333334</v>
       </c>
-      <c r="B97" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C97" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D97" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E97" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F97" s="14"/>
+      <c r="B97" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E97" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F97" s="12"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
@@ -4158,22 +4091,22 @@
       <c r="Z97" s="3"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="18">
-        <v>0.625</v>
-      </c>
-      <c r="B98" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C98" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D98" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E98" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F98" s="14"/>
+      <c r="A98" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C98" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E98" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F98" s="12"/>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
@@ -4199,19 +4132,19 @@
       <c r="A99" s="4">
         <v>0.6666666666666666</v>
       </c>
-      <c r="B99" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C99" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D99" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E99" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F99" s="14"/>
+      <c r="B99" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C99" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E99" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F99" s="12"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
@@ -4237,19 +4170,19 @@
       <c r="A100" s="4">
         <v>0.7083333333333334</v>
       </c>
-      <c r="B100" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C100" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D100" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E100" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F100" s="14"/>
+      <c r="B100" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E100" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F100" s="12"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
@@ -4273,22 +4206,22 @@
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F101" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C101" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D101" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
@@ -4315,21 +4248,19 @@
       <c r="A102" s="4">
         <v>0.375</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B102" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C102" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F102" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="E102" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F102" s="14"/>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
@@ -4355,21 +4286,19 @@
       <c r="A103" s="4">
         <v>0.4166666666666667</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B103" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D103" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C103" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F103" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="E103" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F103" s="14"/>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
@@ -4395,21 +4324,19 @@
       <c r="A104" s="4">
         <v>0.4583333333333333</v>
       </c>
-      <c r="B104" s="5" t="s">
-        <v>6</v>
+      <c r="B104" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D104" s="7" t="s">
-        <v>8</v>
+      <c r="D104" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F104" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="F104" s="14"/>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
@@ -4435,21 +4362,19 @@
       <c r="A105" s="4">
         <v>0.5</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>6</v>
+      <c r="B105" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D105" s="7" t="s">
-        <v>8</v>
+      <c r="D105" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="E105" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F105" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="F105" s="14"/>
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
@@ -4473,11 +4398,11 @@
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="10"/>
-      <c r="B106" s="12"/>
-      <c r="C106" s="20"/>
+      <c r="B106" s="11"/>
+      <c r="C106" s="11"/>
       <c r="D106" s="12"/>
-      <c r="E106" s="12"/>
-      <c r="F106" s="11"/>
+      <c r="E106" s="11"/>
+      <c r="F106" s="14"/>
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
@@ -4503,21 +4428,19 @@
       <c r="A107" s="4">
         <v>0.5833333333333334</v>
       </c>
-      <c r="B107" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C107" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D107" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E107" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F107" s="19" t="s">
-        <v>71</v>
-      </c>
+      <c r="B107" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C107" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E107" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F107" s="14"/>
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
@@ -4540,24 +4463,22 @@
       <c r="Z107" s="3"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="18">
-        <v>0.625</v>
-      </c>
-      <c r="B108" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C108" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D108" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E108" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F108" s="19" t="s">
-        <v>71</v>
-      </c>
+      <c r="A108" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C108" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E108" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F108" s="14"/>
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
@@ -4583,21 +4504,19 @@
       <c r="A109" s="4">
         <v>0.6666666666666666</v>
       </c>
-      <c r="B109" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C109" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D109" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E109" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F109" s="19" t="s">
-        <v>71</v>
-      </c>
+      <c r="B109" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E109" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F109" s="14"/>
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
@@ -4623,21 +4542,19 @@
       <c r="A110" s="4">
         <v>0.7083333333333334</v>
       </c>
-      <c r="B110" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C110" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D110" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E110" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F110" s="19" t="s">
-        <v>71</v>
-      </c>
+      <c r="B110" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C110" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D110" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E110" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F110" s="14"/>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
@@ -4661,22 +4578,22 @@
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E111" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B111" s="9" t="s">
+      <c r="F111" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C111" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D111" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E111" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F111" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
@@ -4703,17 +4620,21 @@
       <c r="A112" s="4">
         <v>0.375</v>
       </c>
-      <c r="B112" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C112" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D112" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E112" s="12"/>
-      <c r="F112" s="12"/>
+      <c r="B112" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
@@ -4739,17 +4660,21 @@
       <c r="A113" s="4">
         <v>0.4166666666666667</v>
       </c>
-      <c r="B113" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C113" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D113" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E113" s="12"/>
-      <c r="F113" s="12"/>
+      <c r="B113" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
@@ -4775,17 +4700,21 @@
       <c r="A114" s="4">
         <v>0.4583333333333333</v>
       </c>
-      <c r="B114" s="7" t="s">
+      <c r="B114" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C114" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D114" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E114" s="12"/>
-      <c r="F114" s="12"/>
+      <c r="E114" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
@@ -4811,17 +4740,21 @@
       <c r="A115" s="4">
         <v>0.5</v>
       </c>
-      <c r="B115" s="7" t="s">
+      <c r="B115" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D115" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C115" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D115" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E115" s="12"/>
-      <c r="F115" s="12"/>
+      <c r="E115" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
@@ -4845,10 +4778,10 @@
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="10"/>
-      <c r="B116" s="11"/>
-      <c r="C116" s="11"/>
-      <c r="D116" s="16"/>
-      <c r="E116" s="11"/>
+      <c r="B116" s="12"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
       <c r="F116" s="11"/>
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
@@ -4875,20 +4808,20 @@
       <c r="A117" s="4">
         <v>0.5833333333333334</v>
       </c>
-      <c r="B117" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C117" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D117" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E117" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F117" s="19" t="s">
-        <v>71</v>
+      <c r="B117" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C117" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D117" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E117" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F117" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
@@ -4912,23 +4845,23 @@
       <c r="Z117" s="3"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="18">
-        <v>0.625</v>
-      </c>
-      <c r="B118" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C118" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D118" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E118" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F118" s="19" t="s">
-        <v>71</v>
+      <c r="A118" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C118" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D118" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E118" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F118" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
@@ -4955,20 +4888,20 @@
       <c r="A119" s="4">
         <v>0.6666666666666666</v>
       </c>
-      <c r="B119" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C119" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D119" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E119" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F119" s="19" t="s">
-        <v>71</v>
+      <c r="B119" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C119" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D119" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E119" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F119" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
@@ -4995,20 +4928,20 @@
       <c r="A120" s="4">
         <v>0.7083333333333334</v>
       </c>
-      <c r="B120" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C120" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D120" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E120" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F120" s="19" t="s">
-        <v>71</v>
+      <c r="B120" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C120" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D120" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E120" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F120" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
@@ -5032,6 +4965,24 @@
       <c r="Z120" s="3"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
+      <c r="A121" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
@@ -5054,6 +5005,20 @@
       <c r="Z121" s="3"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
+      <c r="A122" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D122" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E122" s="12"/>
+      <c r="F122" s="12"/>
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
@@ -5076,6 +5041,20 @@
       <c r="Z122" s="3"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
+      <c r="A123" s="4">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E123" s="12"/>
+      <c r="F123" s="12"/>
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
@@ -5098,6 +5077,20 @@
       <c r="Z123" s="3"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
+      <c r="A124" s="4">
+        <v>0.4583333333333333</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C124" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D124" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E124" s="12"/>
+      <c r="F124" s="12"/>
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
@@ -5120,6 +5113,20 @@
       <c r="Z124" s="3"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
+      <c r="A125" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C125" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D125" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
@@ -5142,6 +5149,12 @@
       <c r="Z125" s="3"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
+      <c r="A126" s="10"/>
+      <c r="B126" s="11"/>
+      <c r="C126" s="11"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="11"/>
+      <c r="F126" s="11"/>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
@@ -5164,6 +5177,24 @@
       <c r="Z126" s="3"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
+      <c r="A127" s="4">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="B127" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C127" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D127" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E127" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F127" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
@@ -5186,6 +5217,24 @@
       <c r="Z127" s="3"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
+      <c r="A128" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B128" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C128" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D128" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E128" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F128" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
@@ -5208,6 +5257,24 @@
       <c r="Z128" s="3"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
+      <c r="A129" s="4">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="B129" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C129" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D129" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E129" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F129" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
@@ -5230,6 +5297,24 @@
       <c r="Z129" s="3"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
+      <c r="A130" s="4">
+        <v>0.7083333333333334</v>
+      </c>
+      <c r="B130" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D130" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E130" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F130" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
@@ -11627,9 +11712,6 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>